<commit_message>
add aicharacter 500 nd 501
</commit_message>
<xml_diff>
--- a/test_cases/PE-16_TC-04_CreateAccountInvalidAICharacterLimit499.xlsx
+++ b/test_cases/PE-16_TC-04_CreateAccountInvalidAICharacterLimit499.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nico\Escritorio\.UADE\TESTING\TestingAplicaciones-Smere-TPO\test_cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fuckultad\testin\tpo\TestingAplicaciones-Smere-TPO\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA53801D-98D8-4E85-8AC5-BB7EA26AF410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1EFAE8-3801-4A30-BFAE-6005CBB89DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -192,21 +192,12 @@
     <t>Click register button</t>
   </si>
   <si>
-    <t>Create Account - Invalid date of birth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify additional information field's character limit entering 499 characters </t>
-  </si>
-  <si>
     <t>User is correctly registered</t>
   </si>
   <si>
     <t>Date of birth 01/01/2004</t>
   </si>
   <si>
-    <t>Additional information = Big windLorem ipsum dolor sit amet, consectetur adipiscing elit. Vivamus varius, ex eu elementum gravida, mauris nisi scelerisque quam, tempor dapibus orci quam ultricies lacus. Suspendisse dapibus, nibh sed pharetra accumsan, dolor ligula varius ante, a rutrum justo mi fringilla nunc. Lorem ipsum dolor sit amet, consectetur adipiscing elit. Duis dui velit, commodo vel lectus in, mollis porta elit. Quisque interdum leo purus, vitae fringilla risus tincidunt quis. Pellentesque fringilla nisi quis diam  owed building on the corner</t>
-  </si>
-  <si>
     <t>Password = Passtest1!</t>
   </si>
   <si>
@@ -214,6 +205,15 @@
   </si>
   <si>
     <t>TC-16-04</t>
+  </si>
+  <si>
+    <t>Additional information = Big windLorem ipsum dolor sit amet, consectetur adipiscing elit. Vivamus varius, ex eu elementum gravida, mauris nisi scelerisque quam, tempor dapibus orci quam ultricies lacus. Suspendisse dapibus, nibh sed pharetra accumsan, dolor ligula varius ante, a rutrum justo mi fringilla nunc. Lorem ipsum dolor sit amet, consectetur adipiscing elit. Duis dui velit, commodo vel lectus in, mollis porta elit. Quisque interdum leo purus, vitae fringilla risus tincidunt quis. Pellentesque fringilla nisi quis diam  owed building on the corner.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify additional information field's character limit entering 500 characters </t>
+  </si>
+  <si>
+    <t>Create Account - Additional Information Character Limit</t>
   </si>
 </sst>
 </file>
@@ -708,89 +708,89 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1079,7 +1079,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="H1" sqref="H1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,25 +1096,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="39"/>
+      <c r="D1" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="28"/>
       <c r="F1" s="14"/>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
+      <c r="H1" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
@@ -1124,21 +1124,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="54"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="49"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="38"/>
       <c r="L2" s="14"/>
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
@@ -1147,8 +1147,8 @@
       <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="17" t="s">
         <v>5</v>
       </c>
@@ -1159,10 +1159,10 @@
       <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="52"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1203,14 +1203,14 @@
       <c r="G5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="33" t="s">
+      <c r="I5" s="47"/>
+      <c r="J5" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="34"/>
+      <c r="K5" s="49"/>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
@@ -1225,14 +1225,14 @@
       <c r="G6" s="10">
         <v>1</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="36" t="s">
+      <c r="I6" s="52"/>
+      <c r="J6" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="37"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
@@ -1255,14 +1255,14 @@
       <c r="G7" s="10">
         <v>2</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="36" t="s">
+      <c r="I7" s="52"/>
+      <c r="J7" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="37"/>
+      <c r="K7" s="52"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -1285,14 +1285,14 @@
       <c r="G8" s="10">
         <v>3</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="37"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="52"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
@@ -1353,7 +1353,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="14"/>
@@ -1373,7 +1373,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -1416,16 +1416,16 @@
         <v>40</v>
       </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="50" t="s">
+      <c r="G14" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
     </row>
     <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
@@ -1438,22 +1438,22 @@
         <v>41</v>
       </c>
       <c r="F15" s="14"/>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35" t="s">
+      <c r="H15" s="50"/>
+      <c r="I15" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35" t="s">
+      <c r="J15" s="50"/>
+      <c r="K15" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35" t="s">
+      <c r="L15" s="50"/>
+      <c r="M15" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="35"/>
+      <c r="N15" s="50"/>
     </row>
     <row r="16" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
@@ -1466,22 +1466,22 @@
         <v>42</v>
       </c>
       <c r="F16" s="14"/>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="29" t="s">
+      <c r="H16" s="45"/>
+      <c r="I16" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="29" t="s">
+      <c r="J16" s="45"/>
+      <c r="K16" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="30"/>
-      <c r="M16" s="29" t="s">
+      <c r="L16" s="45"/>
+      <c r="M16" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="30"/>
+      <c r="N16" s="45"/>
     </row>
     <row r="17" spans="1:14" ht="39" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
@@ -1561,7 +1561,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="7" t="s">
@@ -1692,22 +1692,22 @@
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="28" t="s">
+      <c r="G25" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28" t="s">
+      <c r="H25" s="53"/>
+      <c r="I25" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28" t="s">
+      <c r="J25" s="53"/>
+      <c r="K25" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28" t="s">
+      <c r="L25" s="53"/>
+      <c r="M25" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="28"/>
+      <c r="N25" s="53"/>
     </row>
     <row r="26" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
@@ -1716,16 +1716,16 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27" t="s">
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
@@ -1734,14 +1734,14 @@
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
@@ -1750,14 +1750,14 @@
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="54"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
@@ -1766,14 +1766,14 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
@@ -1782,24 +1782,41 @@
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:K2"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
@@ -1816,30 +1833,13 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:K2"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>